<commit_message>
Update cost data in Costi_ingredienti.xlsx for improved potion processing
</commit_message>
<xml_diff>
--- a/backend/data/Costi_ingredienti.xlsx
+++ b/backend/data/Costi_ingredienti.xlsx
@@ -130,7 +130,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -143,7 +143,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -224,26 +224,23 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +562,10 @@
     <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,7 +584,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -606,7 +603,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -625,7 +622,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -644,7 +641,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -663,7 +660,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -682,7 +679,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -701,7 +698,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -720,7 +717,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -758,7 +755,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -777,7 +774,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
@@ -815,7 +812,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -834,7 +831,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -853,7 +850,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -872,7 +869,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -891,7 +888,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -910,7 +907,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
@@ -929,7 +926,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
@@ -967,7 +964,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
@@ -986,7 +983,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1024,7 +1021,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1062,7 +1059,7 @@
       <c r="L26" s="10"/>
       <c r="M26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1082,9 @@
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="12">
+        <v>0.2</v>
+      </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1102,7 +1101,9 @@
       <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="12">
+        <v>0.2</v>
+      </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1119,7 +1120,9 @@
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="12">
+        <v>0.4</v>
+      </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>

</xml_diff>

<commit_message>
Add potion processing interface with ingredient selection and calculation features
</commit_message>
<xml_diff>
--- a/backend/data/Costi_ingredienti.xlsx
+++ b/backend/data/Costi_ingredienti.xlsx
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,12 +138,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -222,9 +216,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -550,19 +541,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -1048,15 +1039,15 @@
         <v>0.3333</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -1082,7 +1073,7 @@
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="11">
         <v>0.2</v>
       </c>
       <c r="C28" s="4"/>
@@ -1101,7 +1092,7 @@
       <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="11">
         <v>0.2</v>
       </c>
       <c r="C29" s="4"/>
@@ -1120,7 +1111,7 @@
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="11">
         <v>0.4</v>
       </c>
       <c r="C30" s="4"/>
@@ -1135,9 +1126,9 @@
       <c r="L30" s="4"/>
       <c r="M30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A31" s="4"/>
-      <c r="B31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1150,9 +1141,9 @@
       <c r="L31" s="4"/>
       <c r="M31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A32" s="4"/>
-      <c r="B32" s="12"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1165,9 +1156,9 @@
       <c r="L32" s="4"/>
       <c r="M32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A33" s="4"/>
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1180,9 +1171,9 @@
       <c r="L33" s="4"/>
       <c r="M33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="12"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>

</xml_diff>